<commit_message>
Working version of a dispatcher
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/REFrameworkNET5/StudioTemplates/REFramework/contentFiles/any/any/pt2/VisualBasic/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasyu\Documents\UiPath\Advertisement Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4545" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +84,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -160,13 +156,31 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>OLXAdvertisementDispatcher</t>
+  </si>
+  <si>
+    <t>OLX_URL</t>
+  </si>
+  <si>
+    <t>https://www.olx.ua/</t>
+  </si>
+  <si>
+    <t>OLX_Search_Item</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>SearchPeriod</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +204,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,10 +228,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -221,9 +242,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Гіперпосилання" xfId="1" builtinId="8"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -534,19 +557,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -585,40 +608,61 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1610,25 +1654,28 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1712,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1673,18 +1720,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1755,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1777,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1788,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1799,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2779,17 +2826,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2800,7 +2849,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>